<commit_message>
Se conecto la logica del Scraper de Horoscopos con la API, se habilito una nueva ruta de consulta de datos, faltan corregir los formatos
</commit_message>
<xml_diff>
--- a/Scraper/predicciones.xlsx
+++ b/Scraper/predicciones.xlsx
@@ -87,85 +87,85 @@
   <si>
     <t xml:space="preserve">
 PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Cuando la gente habla un idioma distinto al nuestro, nos resulta difícil entender lo que dicen. Observar atentamente las expresiones faciales y los gestos ayuda. Algunas palabras pueden ser similares, mientras que otras, que suenan igual, pueden tener significados completamente diferentes. Es entonces cuando podemos equivocarnos y traducir mal. Igual que ocurre con las palabras, ocurre con las experiencias. Las más complicadas son las que pensamos que sabemos manejar... ¡aunque no sea ése el caso! Este fin de semana tómate tu tiempo para comprender bien lo que esté ocurriendo. No saques conclusiones precipitadas.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Eres una decidida nativa de Tauro. Por difícil que sea el reto o largo que sea el viaje, tu instinto es seguir adelante. Si llevas a cuestas una gran responsabilidad, antes prefieres seguir luchando que desentenderte de ella. Lo cual es noble... pero quizás un poco imprudente. Esta semana tienes que ir a tu ritmo. A veces (sólo a veces) eso significa decirle a la gente que no puedes hacer lo que esperan que hagas. Quiere decir defraudar ahora un poco a otra persona para no tener que defraudarla mucho en el futuro. Ha llegado el momento de cuidar de ti misma.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Ya sea a propósito o sin querer, tu confianza se ha visto minada. Esto está distorsionando lo que piensas de una situación de tal manera que estás viendo problemas incluso donde no los hay. Lo que aumenta tu incertidumbre. ¡Maldición! Lo irónico es que todo marcha a la perfección. El problema al que te estás enfrentando es justo lo que necesitas para poder tomar una buena decisión sobre tu futuro. Esta semana te brinda una revisión de la realidad y un cambio de perspectiva. Puedes dejar de preocuparte y estar más segura de ti misma.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Si te gusta llevar una vida tranquila, ¿por qué pasas tiempo con "tú ya sabes quién"? Y, ya que estamos, ¿por qué pasas tiempo haciendo "tú ya sabes qué"? Y, ahora que nos hemos puesto a pensarlo realmente, ¿por qué te atrae tanto esa loca idea... tú ya sabes cuál? No se trata de revelar tus secretos. La cosa va de recordarte que, siendo realistas, no quieres una vida tranquila. Te gusta la emoción. Y encuentras la manera de traerla a tu mundo. Si esta semana sabes muy bien lo que realmente quieres, tendrás muchas posibilidades de conseguirlo.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-¿Estás preparada para una sorpresa? Como Venus está en tu signo, conectando con el estrafalario Urano, una fuerza profundamente positiva entrará de sopetón en tu vida. ¿Supondrá un avance definitivo en su vida amorosa? Parece muy probable. Aunque no dé la impresión de estar directamente relacionado con el amor, sí que tiene que ver con algo que llevas mucho tiempo deseando tener en tu mundo y que traerá placer a tu vida. Esta semana acepta cualquier cambio que se te presente. Las semillas de esperanza que plantes te deleitarán rápidamente con las hermosas oportunidades que te brindarán.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-En lugar de pedir lo que crees que puedes conseguir, prueba a pedir lo que realmente quieres. El hecho de que seas una práctica nativa de Virgo no significa que tengas que limitarte a elegir con pragmatismo. Sólo tienes que fijarte objetivos prácticos cuando hayas demostrado que no se gana nada siendo idealista. Y aún no has terminado de explorar tus opciones. Vale la pena que reivindiques tu sueño. Intenta alcanzar el objetivo más prometedor que puedas imaginar. ¿Por qué renunciar a un ideal que podría acabar siendo posible?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-¿Qué que te gustaría que te dijera acerca de la semana que tienes por delante? ¿Hay algún deseo que esperas que se cumpla? ¿Qué me dices del sueño que te gustaría que formase parte de tu realidad? Seguro que no necesitas que te tranquilice, ¿no? ¿No confías en que puedas hacer que eso ocurra? Deberías confiar en ti. Estás en una posición poderosa. El vínculo que forman Venus, tu regente, y Urano pone de manifiesto tus cualidades intuitivas y te da la visión que necesitas para emprender acciones significativas. Tienes el éxito tan cerca (o tan lejos) como lo esté tu capacidad para creer en ti misma.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Crees que una historia complicada ha llegado a su conclusión. Ya has oído todo lo que había que oír. Ya no te esperan más sorpresas. Aunque no estás especialmente contenta con el resultado, lo has aceptado. Estás preparada para hacer lo que haga falta para vivir con la nueva realidad. Pero echas en falta una información clave. Varios factores que se te habían pasado por alto, están a punto de salir a la luz. Una visión más inspiradora de un aspecto de tu pasado te ayudará este fin de semana a construir un futuro prometedor.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Cierto aspecto de tu vida necesita una revisión. Ha durado demasiado tiempo. Ya no es tan interesante (ni tan gratificante). Has estado intentando justificar los actos de ciertas personas y soportando una situación muy complicada para ti. En lugar de preguntarte por qué te has metido en esto, céntrate en lo que puedes hacer para cambiarlo. Como el Sol se vincula a Júpiter, tu regente, se te está bendiciendo con el poder de darte a valer, ponerte firme, tener claro lo que quieres y estar segura de cómo lo vas a conseguir. Tiene pinta de ser una semana satisfactoria y productiva.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Está claro que cruzar la línea de meta por delante de los demás es gratificante. Pero compartir el éxito con alguien a tu lado, es aún más satisfactorio. Los triunfos personales pueden llegar a ser solitarios. Las victorias que provienen de haber trabajado con otras personas crean vínculos que perduran en el tiempo. Puede que tengas la sensación de que tu participación en un proyecto es relativamente insignificante. Pero estás desempeñando un papel fundamental en un proceso importante. La inminente recompensa celestial lleva tu nombre y el de otras personas. Has trabajado duro. Te has ganado el reconocimiento.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-¿Qué deseo secreto guardas en lo más profundo de tu corazón? Si pudieras provocar un cambio que trajera más felicidad a tu mundo, ¿qué cambiarías? Sé totalmente sincera. Si tú misma te engañas, reducirás las posibilidades de beneficiarte de los regalos que te brinda el cosmos esta semana. Puede que sin darte cuenta eches por tierra la posibilidad de maximizar las oportunidades que se te presenten. Si expresas tus sentimientos, como Urano, tu regente, se vincula a Venus (amor y placer), encontrarás apoyo donde menos te lo esperes y eso te ayudará a hacer realidad un sueño.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-PredicciÃ³n
-                        para hoy                        06 de Agosto de 2023
-Es fácil pensar que estamos rodeados de gente mejor informada y con más experiencia que nosotros. Como pensamos que esas personas lo saben todo, vamos con pies de plomo para aseguramos de que no hacemos nada que parezca una tontería. Lo que pasa realmente es que el mundo está lleno de gente a la que le pone igual de nerviosa la idea de que la pillen cometiendo algún error. Así que suelen ocultan sus temores tras cortinas de humo de poder y opinión. Esta semana tendrás una información que a cierta persona podría resultarle difícil de escuchar. Decir lo que piensas te sentará bien... y hará que ganes respeto.
+                        para hoy                        07 de Agosto de 2023
+Algunas personas tienen que pedir prestado con pocas esperanzas de que puedan llegar a cancelar su deuda. Es extrañamente irónico que la gente con las mejores puntuaciones de crédito suela ser la que no necesita ayuda adicional. Cuando se trata de cuestiones sociales y emocionales, algunos hacemos promesas que nunca seremos capaces de cumplir, mientras que otros mantienen promesas que no deberían haber hecho nunca. Tienes derecho a recibir ayuda. Pero tienes que pedirla para obtenerla. Si lo haces, debes saber que tu petición será atendida. Aprovecha al máximo los regalos que te lleguen... puedes corresponder siempre a la amabilidad.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Tendemos a descartar el soñar despiertos como una pérdida de tiempo y energía. ¿Qué sentido tiene matar el tiempo perdidos en fantasías que no se harán realidad? ¿No sería mejor que invirtiésemos nuestros pensamientos en cuestiones más pragmáticas? Sin embargo, a veces es esencial dejar volar la imaginación. Creamos visiones de cómo "podrían" ser las cosas, y a partir de eso dar los pasos necesarios para hacer que esas visiones formen parte de nuestra realidad. Hoy hay una pizca de polvo de hadas en el aire. Así que no descartes una idea descabellada. Podría dar un cambio en las reglas del juego.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Incluso en esos lugares del mundo en los que el clima es predecible, el tiempo es una fuente de conversación. Todos lo utilizamos para romper el hielo y entablar conversaciones con la gente. Y no tienen por qué ser conversaciones de importancia para ser agradables y gratificantes; a veces, hablar del tiempo que está haciendo basta para crear en nosotros la sensación de que realmente nos relacionamos con el mundo. Y esto puede abrir además la puerta a conversaciones sobre temas más personales. Hoy puede surgir una idea importante de un intercambio trivial. Estate abierta a ello.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+No estás muy contenta con el comportamiento de cierta persona. Estás asombrada... incluso escandalizada. ¿Cómo se atreve a actuar de una manera tan egoísta? Sus acciones han afectado a la vida y el bienestar de otras personas, y eso ha hecho que te enfades. Pero tomarte tan a pecho estas emociones no va a ayudar a nadie. Si las dejas a un lado, tendrás más claro qué puedes hacer para mejorar esta situación. El vínculo que forman hoy el Sol y Júpiter te recuerda que tienes poder para lograr un cambio positivo. Puedes utilizar la fuerza de tus sentimientos para fomentar la reconciliación.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+“Ojalá... Debería haber... ¿Por qué no...?” Todos hemos pasado por eso. En un momento u otro, todos miramos atrás con arrepentimiento, ante una decisión pasada. Pero nuestros errores son herramientas de aprendizaje. Cuando los analizamos correctamente, nos ayudan a comprender cosas nuevas. Y siempre podemos enmendar los errores del pasado. Alguien de tu entorno podría apreciar la oportunidad de pedir perdón por una acción de la que se arrepiente. Como el Sol, tu regente, está vinculado a Júpiter, si alargas la mano en señal de amistad, es posible un nuevo comienzo.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Imagínate que cada vez que volvemos de un viaje, antes de ser recibidos de nuevo en nuestros hogares y lugares de trabajo, tuviésemos que introducir una contraseña o un número PIN y pasar el control de seguridad. ¡Espantoso! Por suerte, y a pesar de que ciertos frikis de la tecnología parecen dudar de la capacidad humana de reconocerse con sólo mirarse a la cara, ¡eso nunca ocurrirá! Algo irritante se interpone entre tú y un objetivo que tienes al alcance de la mano. Tienes que cumplir una serie de molestos e innecesarios protocolos. Pero una vez que ya están cumplidos, volarás libre.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Imagínate que haces todo lo posible por conseguir la semilla de una valiosa flor poco común. La plantas, abonas y riegas la tierra, pero no ocurre nada. ¿Qué haces? ¿Arrancarla y comprarte un ramo? ¿O prepararte para tener paciencia? Tienes un plan. Puede que no tengas claro el tiempo que tardará en dar frutos. Tal vez no estés segura de que vaya a llegar a buen término. Pero intuyes que encierra la semilla de algo. Confía en ese instinto. Aunque podría pasar un tiempo antes de que florezca por completo, si no pierdes el optimismo y buscas señales de esperanza, pronto aparecerán.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+No nos quedemos nunca sin motivos para estar enfadados, impacientes o frustrados. Por suerte tampoco se nos acaban las razones para ser considerados, empáticos o indulgentes. Si fuésemos siempre perfectos, probablemente la vida sería aburrida. Y si permitiésemos que nuestros rencores e inquietudes dominen nuestros pensamientos y sentimientos, la vida sería deprimente. En los últimos días te las has tenido que ver con una buena dosis de problemas. Sin embargo, el día de hoy te trae un momento de inspiración y una buena noticia. Algo maravilloso está ocurriendo. Tu estado de ánimo está a punto de mejorar.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+La gente se siente atraída hacia ti. Hay algo en tu entusiasmo que resulta atractivo. Y esto significa que algunas veces atraes a las compañías que no te convienen. Tu reto consiste en distinguir entre la gente que es digna de tu tiempo y la que viene a disfrutar de tu luz. Como el Sol se vincula a Júpiter, tu regente, debes elegir con quién quieres compartir tus pensamientos más íntimos. Si no das demasiado de ti, atraerás a la gente que quiere saber más de tu auténtico yo. Son las personas que realmente necesitas en tu mundo.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+No necesitamos estar hasta arriba de ideas nuevas para tener una buena conversación. A veces es agradable repetir algo de lo que ya habíamos hablado antes. Es como si siguiésemos un guión, sabemos lo que vamos a decir y cuál va a ser la respuesta. Resulta tranquilizador y reconfortante. Esto funciona bien cuando todos los participantes están contentos con el tema de conversación. Pero no es tan agradable cuando se está hablando de algo que cause dolor o problemas.  Hoy, con unas pocas palabras inequívocas, podrás trasladar una situación difícil a un espacio mejor y más saludable desde el que sea posible una reconciliación.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Eres famosa por tu tendencia a analizar las situaciones. Aunque a veces la gente se burle de ti por el tiempo que tardas en tomar una decisión importante, admiran tu capacidad para saber elegir bien (y aferrarte firmemente a lo que hayas decidido). Para poder tomar una buena decisión, necesitas toda la información disponible. La conjunción que forman hoy el Sol y Júpiter aporta un dato esencial que se te estaba pasando por alto. En cuanto hayas encajado esa información en lo que ya has descubierto, podrás actuar. La decisión que estás a punto de tomar está bien fundada... y es genial.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PredicciÃ³n
+                        para hoy                        07 de Agosto de 2023
+Me pregunto quién inició el mito de que el poder es atractivo. Seguro que fue alguien que estuvo en una posición de poder. Es el tipo de idea errónea que sólo podría hacer circular alguien que intentase cubrir su comportamiento con un velo de misterio. Lo que sí sabemos con certeza, es que el poder corrompe. Entonces, ¿debería preocuparte el poder que está llegando a tu vida? Conforme el Sol se alinea con Júpiter, tienes la oportunidad de recuperar el control del equilibrio dentro de una relación. Sólo tienes que asegurarte de hacer que la generosidad y la justicia sean los principios de este nuevo comienzo.
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Horoscopo 9 de Agosto
</commit_message>
<xml_diff>
--- a/Scraper/predicciones.xlsx
+++ b/Scraper/predicciones.xlsx
@@ -62,63 +62,63 @@
   </si>
   <si>
     <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Si la historia de Adan y Eva se repusiera en el mundo actual, lo que causaria nuestra perdicion no seria el deseo de una manzana (o granada, segun a quien escuches). Seria un coche nuevo !o un televisor de ultima generacion! Aun seguimos queriendo lo que no podemos tener. Deseamos la ultima version, lo mejor, lo que esta mas de moda. Pero todo acaba siendo sustituido por un nuevo modelo. Y, a pesar del habil marketing, poseer los mejores productos no da la felicidad. Algo precioso se esconde hoy en la monotonia.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Tienes un monton de razones para sentirte orgullosa de ti misma y de lo que has conseguido. Has sabido manejarte bien en una situacion dificil. Aunque no te las hayas arreglado para resolverla del todo, has calmado las cosas. Es dificil imaginar como alguien podria haberlo hecho mejor. Pero la parte que sigue sin resolver aun te esta molestando. Y estas bajo presion para solucionarla. Es cierto que te faltan recursos. No te vendria mal tener mas apoyo. Si hoy tienes fe en ti misma, veras lo que hay que hacer. Podras acceder a lo que necesitas.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Nos resulta inquietante no saber algo. Asi que seguimos haciendo preguntas, obteniendo respuestas y volviendo a preguntar despues. De forma parecida seguimos en nuestra vida unos patrones familiares. Nos levantamos de la cama, nos cansamos y volvemos a dormir. Y repetimos estas rutinas sin cesar. Asi es como funciona la vida. ?Nos sentimos frustrados porque la gran cena que comimos la noche pasada no nos saciara hasta el fin de semana? Pues no. Lo aceptamos. Tal vez te frustre repetir un ejercicio y puede que te resulte dificil encontrar una solucion. Pero estas satisfaciendo una necesidad importante.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Resulta que algo que deberia ser sencillo y sin complicaciones esta lleno de trampas. Da mucha rabia. No puedes hacer esto... porque, si lo haces, ocurrira aquello. No puedes hacer eso. O eso. O eso. !Que fastidio! O mas bien si puedes hacerlo, pero las consecuencias que esto trae no parecen especialmente atractivas. ?Que se supone que debes hacer? Si en lugar de quedarte pasmada investigas esta situacion mas a fondo, veras que solo hay un problema que resolver. Y la buena noticia es que solo hay una solucion ante ti. Y mira por donde, es la correcta.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-El dicho "el diagnostico es la mitad del remedio" no solo se aplica a los problemas medicos. Sea cual sea el problema al que nos enfrentemos, si nos tomamos tiempo para identificarlo, podremos empezar a abordarlo. Pero el diagnostico debe centrarse en el meollo de la situacion. Si se basa en una idea preconcebida, no conducira al remedio adecuado. Tienes problemas porque estas basando un plan de accion en una suposicion. Si lo pones en duda, sabras como abordarlo exactamente y de una manera que hara que te sientas capacitada para solucionarlo satisfactoriamente y sin problemas.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-?Que sentido tiene que te compliques la vida (o se la compliques a los demas)? ?Que tiene de malo quedarte con la opcion facil? Como concienzuda nativa de Virgo, tienes habilidad de sobra para enfrentarte a situaciones dificiles. Estas a la altura de las circunstancias. ?Es esa la razon de que tengas dificultades para aprovechar la oportunidad que se te ofrece? Por supuesto que es prudente comprobar si hay inconvenientes ocultos. Pero no olvides que algunas veces la vida nos trae cosas buenas. Y que a veces funcionan sorprendentemente bien. Hoy la opcion facil es una buena opcion. Te la mereces.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Por muy insegura que pudieras sentirte al entrar en un nuevo capitulo de tu vida, ten por seguro que el cosmos confia en ti. No solo esta seguro de que estas haciendo lo correcto, sino que hace todo lo posible para que tu tambien lo sepas. Las senales del camino son tan grandes que es dificil ignorarlas. Tus dudas se deben a que no te resulta facil dejar algo atras (aunque no funcione). Pero el camino parece claro y atractivo. Te lleva a un destino que hara que seas mas feliz. Da el paso. No te arrepentiras.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Algunas personas tienen tanto dinero en su cuenta bancaria que pueden permitirse gastar una fortuna en cosas que se pueden adquirir por la mitad de precio. Si el dinero es suyo, por supuesto que estan en su derecho de gastarselo como quieran. Si no lo es, sin duda merecen ser rescatados de su estado de ignorancia, ?no? Puede que no sea un problema financiero, pero ?no estaras invirtiendo mas de la cuenta en algo que podrias encontrar en otra parte, a un "coste" menor? Hoy puedes tomar una decision que te libere de una costosa exigencia de tu tiempo y energia.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-El arte de hacer reir a la gente incluye algo mas que encontrar cosas divertidas que contar. Como saben los buenos comicos, tiene que ver con la manera en que se cuenta el chiste. La sincronizacion lo es todo. El estilo es tan importante como la sustancia. ?Por que te estoy hablando de comedia cuando tienes entre manos un tema serio? Hoy no necesitas contar un chiste pero si compartir una informacion importante sobre como te sientes. Y esto te esta resultando dificil. Si eliges el momento oportuno con cuidado, podras dar la noticia de forma agradable.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Es en los momentos de calma y tranquilidad cuando percibimos la mano de la serendipia influyendo en nuestra vida. Pero cuando nos estamos esforzando para hacer frente al caos de nuestro mundo, algunas veces se producen coincidencias. A causa de que siempre pueden ocurrir cosas buenas, resulta mas dificil evaluar lo bien que nos va la vida y, el hecho de que supongan un desafio, no significa que las cosas vayan mal. Las influencias cosmicas indican que estas a punto de experimentar una sensacion de exaltacion e inspiracion. Te ayudara a ver por que un camino complicado es menos dificil de lo que parece.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Desde la dieta paleo hasta la alimentacion basada en productos vegetales, la enorme cantidad de recomendaciones dieteticas complica mucho saber comer sano. Lo que funciona para unas personas no lo hace para otras. Ni siquiera los expertos se ponen de acuerdo sobre cuales son los mejores alimentos. Si no tenemos cuidado, elegir entre lo "bueno" y lo "malo" aumenta nuestro nivel de estres. Y todos sabemos que eso no es sano. La mejor opcion para ti hoy es elegir el camino que menos te estrese. Si haces lo que te sienta bien, las consecuencias seran positivas.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        08 de Agosto de 2023
-Segun una cancion de Bob Dylan, no hace falta ser meteorologo para saber en que direccion sopla el viento. Sin embargo, el viento puede ser enganoso. Puede cambiar de direccion en un abrir y cerrar de ojos. Por eso los meteorologos son tan utiles. Lo mismo ocurre con los astrologos. En algunas ocasiones sabes lo que va a pasar (y no necesitas orientacion). Pero en otras lees mal las senales (igual que le pasa a todo el mundo). En este preciso momento crees que te enfrentas a un problema de grandes dimensiones. Mi trabajo consiste en asegurarte que puedes resolverlo facilmente.</t>
+                        para hoy                        09 de Agosto de 2023
+Los animales saben comunicarse entre si de una manera que hace que otras criaturas se mantengan alertas ante posibles problemas. El miedo se comunica con facilidad en la naturaleza porque para todos es beneficioso ser conscientes de la necesidad de tomar inmediatamente medidas evasivas. Los humanos conservamos la capacidad primitiva de transmitir esta emocion. Lo cual es estupendo... a menos que nos aqueje un falso temor. Por eso cobran fuerza las ansiedades infundadas. Parece que a la gente de tu mundo le preocupa mucho una situacion determinada. Sin embargo, eso no es razon para dejar que te preocupe.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Aunque se nos anima a que hagamos uso de nuestra imaginacion, acabamos tomando prestada la de los demas. Vemos dramas en la television. Vamos al cine. Nos dejamos influir por los anuncios y compramos los productos que han disenado unos desconocidos para nosotros. Lo malo es que cuanto mas dejamos que las visiones de otras personas marquen el tono de nuestra vida, mas limitada acaba siendo nuestra imaginacion. El hecho de que cierta persona no pueda concebir tu idea de lo que es posible no significa que no debas creer en ella. Como tu regente se vincula al innovador Urano, te sientes inspirada. Ten fe en ti.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Es facil pensar que son las diferencias las que causan los conflictos. Pero estos tienden a surgir de las similitudes. Podemos ser poco exigentes con los desconocidos. La gente cuyo aspecto, modo de actuar o de hablar son distintos a los nuestros tiende a fascinarnos, en vez de enfurecernos. Son aquellas personas que proceden de situaciones parecidas a la nuestra - pero que no opinan igual que nosotros, las que nos sacan de quicio. Las batallas mas dramaticas casi siempre se libran por las cosas mas triviales. Hoy puedes tender un puente hacia cierta persona. Las dos teneis algo en comun que hara avanzar vuestros planes.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+?Hay algun modo de que consigas lo que necesitas sin tener que disgustar a nadie? Quieres contentar a todo el mundo pero sabes muy bien lo que quieres. Entonces, ?que deberias hacer? ?En que tienes que ceder para que todo el mundo se sienta integrado en tus objetivos? Necesitas respuestas para poder seguir adelante con cierta sensacion de tranquilidad y control. Pero no necesitas resolverlo todo hoy. Ni tampoco debes sentirte presionada a aceptar las opiniones de los demas sobre lo que hay que hacer. Por algo estas en el asiento del conductor. Toma el control del volante.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Algunas personas no soportan la idea de no saber algo. Por eso, si se les pregunta algo que no saben, se inventan la respuesta. Hacen conjeturas. Y esto seria aceptable si pronunciaran su suposicion con un tinte de duda en la voz. Pero suelen dar su respuesta en un tono autoritario que no admite discusion. Y cuanto mas fanfarronean, mas categoricos se vuelven. A pesar de tu optimismo, alguien ha hecho todo lo posible para convencerte de que cierta situacion no tiene solucion. Estas a punto de descubrir lo contrario.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Cuando nos ponemos en marcha hacia un nuevo destino, es facil que tomemos una ruta equivocada. ?Deberiamos volver sobre nuestros pasos tan pronto como nos hayamos dado cuenta del error? ?O seguir adelante, confiando en que el cosmos tiene buenas razones para desviarnos? Cuando viajamos por carreteras fisicas, Google Maps puede orientarnos. Cuando se trata de viajes interiores, la ayuda es menos obvia y el camino a seguir no es tan facil de adivinar. Sin embargo, tu intuicion es hoy tan fiable como cualquier navegador por satelite. Si confias en ella, veras senales claras de que vas por buen camino.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Estas detectando los planes ocultos de cierta persona. Un escenario no es lo que parece. Esa persona ha disfrazado habilmente sus intenciones y cada vez que piensas o hablas sobre el tema te das cuenta de ello. Y no eres la unica que percibe esta confusion. De hecho, el aire esta tan cargado de suposiciones que podrias cortarlo con un cuchillo. Por eso hay tanta tension y caos. ?Como puedes aliviar esta incomoda sensacion? Al hablar abiertamente sobre lo que se te niega, podras convertir una situacion delicada en una constructiva.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Te estas preparando psicologicamente, para afrontar un reto. ?Por que a veces la vida es tan dificil? ?Para que esperar tensiones cuando deberias poder mirar al futuro con esperanza? Lo que ocurre es que tu sensibilidad natural esta captando las ansiedades de los demas. Se han puesto a la defensiva y su actitud te esta afectando. Pero si piensas en los aspectos positivos y respondes a sus preocupaciones con carino y amabilidad, ?podras influir en su estado de animo? Claro que puedes. Confia en que todo va a salir bien, porque es lo que va a pasar.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Puesto que es mas facil ganar en las discusiones que ganar amigos, a veces es mejor perder en las primeras para conservar los segundos. Lo que no significa que tengas que echarte atras de un asunto que significa mucho para ti. Pero ser consciente de que alguien siente la misma pasion que tu (pero de otra forma) te ayudara a mantener abiertas las lineas de comunicacion. Si estas abierta a lo que venga y eres generosa, podras ver mas alla de los aciertos y errores de esta situacion. Y encontrar un punto de entendimiento que no pondra en peligro tus creencias.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Dicen que debemos tener cuidado con lo que deseamos... y estan en lo cierto. Algunos suenos son mas gratificantes en teoria que en la realidad. Vistos por fuera parecen sofisticados y exoticos. Vistos por dentro, son muy diferentes. Eso no significa que no debamos intentar ir tras ellos. Pero es mejor que lo hagamos sin gafas de color de rosa que oculten la realidad. Necesitas apoyo para poder satisfacer tu ambicion actual. Si tienes las ideas claras y compartes tus planes con una persona clave, podras avanzar mas deprisa de lo que crees.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Si, como dice la cancion, "la vida no es mas que un sueno", ?que ocurre cuando nos despertamos? ?Nos damos la vuelta en la cama y volvemos a dormir, con un vago recuerdo de lo sonado? ?Que es real y que no lo es? Las respuestas a estas preguntas no son tan claras como te gustaria. En estos momentos estas percibiendo como real cierta preocupacion por el futuro, cuando en realidad solo se trata de una fantasia. Conforme se vincula a Venus, en movimiento retrogrado, Urano, tu regente, te proporciona la capacidad de detectar una ilusion desconcertante. Esto te liberara para que tomes esa decision tan dificil de tomar.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        09 de Agosto de 2023
+Atras quedaron los dias en los que se consideraba que aquellas personas que creian en las hadas y la magia eran unas credulas. Avanzando en el tiempo, no hace mucho se consideraba credula a la gente que creia en el calentamiento global. No es mi intencion transmitir una opinion. Simplemente estoy senalando que, sean cuales sean nuestras teorias y creencias, corremos el riesgo de que se burlen de ellas. Y que cuando una persona a la que valoramos critica nuestros puntos de vista, esto puede hacer que dudemos. Hoy no dejes que te convenzan de algo. Tus ideas estan bien pensadas y son validas. Merecen que obres en consecuencia.</t>
   </si>
   <si>
     <t>https://www.hola.com/horoscopo/aries/</t>

</xml_diff>

<commit_message>
Se agregaron medidas para buscar corregir el formato de los acentos
</commit_message>
<xml_diff>
--- a/Scraper/predicciones.xlsx
+++ b/Scraper/predicciones.xlsx
@@ -62,63 +62,63 @@
   </si>
   <si>
     <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Los animales saben comunicarse entre si de una manera que hace que otras criaturas se mantengan alertas ante posibles problemas. El miedo se comunica con facilidad en la naturaleza porque para todos es beneficioso ser conscientes de la necesidad de tomar inmediatamente medidas evasivas. Los humanos conservamos la capacidad primitiva de transmitir esta emocion. Lo cual es estupendo... a menos que nos aqueje un falso temor. Por eso cobran fuerza las ansiedades infundadas. Parece que a la gente de tu mundo le preocupa mucho una situacion determinada. Sin embargo, eso no es razon para dejar que te preocupe.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Aunque se nos anima a que hagamos uso de nuestra imaginacion, acabamos tomando prestada la de los demas. Vemos dramas en la television. Vamos al cine. Nos dejamos influir por los anuncios y compramos los productos que han disenado unos desconocidos para nosotros. Lo malo es que cuanto mas dejamos que las visiones de otras personas marquen el tono de nuestra vida, mas limitada acaba siendo nuestra imaginacion. El hecho de que cierta persona no pueda concebir tu idea de lo que es posible no significa que no debas creer en ella. Como tu regente se vincula al innovador Urano, te sientes inspirada. Ten fe en ti.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Es facil pensar que son las diferencias las que causan los conflictos. Pero estos tienden a surgir de las similitudes. Podemos ser poco exigentes con los desconocidos. La gente cuyo aspecto, modo de actuar o de hablar son distintos a los nuestros tiende a fascinarnos, en vez de enfurecernos. Son aquellas personas que proceden de situaciones parecidas a la nuestra - pero que no opinan igual que nosotros, las que nos sacan de quicio. Las batallas mas dramaticas casi siempre se libran por las cosas mas triviales. Hoy puedes tender un puente hacia cierta persona. Las dos teneis algo en comun que hara avanzar vuestros planes.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-?Hay algun modo de que consigas lo que necesitas sin tener que disgustar a nadie? Quieres contentar a todo el mundo pero sabes muy bien lo que quieres. Entonces, ?que deberias hacer? ?En que tienes que ceder para que todo el mundo se sienta integrado en tus objetivos? Necesitas respuestas para poder seguir adelante con cierta sensacion de tranquilidad y control. Pero no necesitas resolverlo todo hoy. Ni tampoco debes sentirte presionada a aceptar las opiniones de los demas sobre lo que hay que hacer. Por algo estas en el asiento del conductor. Toma el control del volante.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Algunas personas no soportan la idea de no saber algo. Por eso, si se les pregunta algo que no saben, se inventan la respuesta. Hacen conjeturas. Y esto seria aceptable si pronunciaran su suposicion con un tinte de duda en la voz. Pero suelen dar su respuesta en un tono autoritario que no admite discusion. Y cuanto mas fanfarronean, mas categoricos se vuelven. A pesar de tu optimismo, alguien ha hecho todo lo posible para convencerte de que cierta situacion no tiene solucion. Estas a punto de descubrir lo contrario.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Cuando nos ponemos en marcha hacia un nuevo destino, es facil que tomemos una ruta equivocada. ?Deberiamos volver sobre nuestros pasos tan pronto como nos hayamos dado cuenta del error? ?O seguir adelante, confiando en que el cosmos tiene buenas razones para desviarnos? Cuando viajamos por carreteras fisicas, Google Maps puede orientarnos. Cuando se trata de viajes interiores, la ayuda es menos obvia y el camino a seguir no es tan facil de adivinar. Sin embargo, tu intuicion es hoy tan fiable como cualquier navegador por satelite. Si confias en ella, veras senales claras de que vas por buen camino.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Estas detectando los planes ocultos de cierta persona. Un escenario no es lo que parece. Esa persona ha disfrazado habilmente sus intenciones y cada vez que piensas o hablas sobre el tema te das cuenta de ello. Y no eres la unica que percibe esta confusion. De hecho, el aire esta tan cargado de suposiciones que podrias cortarlo con un cuchillo. Por eso hay tanta tension y caos. ?Como puedes aliviar esta incomoda sensacion? Al hablar abiertamente sobre lo que se te niega, podras convertir una situacion delicada en una constructiva.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Te estas preparando psicologicamente, para afrontar un reto. ?Por que a veces la vida es tan dificil? ?Para que esperar tensiones cuando deberias poder mirar al futuro con esperanza? Lo que ocurre es que tu sensibilidad natural esta captando las ansiedades de los demas. Se han puesto a la defensiva y su actitud te esta afectando. Pero si piensas en los aspectos positivos y respondes a sus preocupaciones con carino y amabilidad, ?podras influir en su estado de animo? Claro que puedes. Confia en que todo va a salir bien, porque es lo que va a pasar.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Puesto que es mas facil ganar en las discusiones que ganar amigos, a veces es mejor perder en las primeras para conservar los segundos. Lo que no significa que tengas que echarte atras de un asunto que significa mucho para ti. Pero ser consciente de que alguien siente la misma pasion que tu (pero de otra forma) te ayudara a mantener abiertas las lineas de comunicacion. Si estas abierta a lo que venga y eres generosa, podras ver mas alla de los aciertos y errores de esta situacion. Y encontrar un punto de entendimiento que no pondra en peligro tus creencias.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Dicen que debemos tener cuidado con lo que deseamos... y estan en lo cierto. Algunos suenos son mas gratificantes en teoria que en la realidad. Vistos por fuera parecen sofisticados y exoticos. Vistos por dentro, son muy diferentes. Eso no significa que no debamos intentar ir tras ellos. Pero es mejor que lo hagamos sin gafas de color de rosa que oculten la realidad. Necesitas apoyo para poder satisfacer tu ambicion actual. Si tienes las ideas claras y compartes tus planes con una persona clave, podras avanzar mas deprisa de lo que crees.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Si, como dice la cancion, "la vida no es mas que un sueno", ?que ocurre cuando nos despertamos? ?Nos damos la vuelta en la cama y volvemos a dormir, con un vago recuerdo de lo sonado? ?Que es real y que no lo es? Las respuestas a estas preguntas no son tan claras como te gustaria. En estos momentos estas percibiendo como real cierta preocupacion por el futuro, cuando en realidad solo se trata de una fantasia. Conforme se vincula a Venus, en movimiento retrogrado, Urano, tu regente, te proporciona la capacidad de detectar una ilusion desconcertante. Esto te liberara para que tomes esa decision tan dificil de tomar.</t>
-  </si>
-  <si>
-    <t>PredicciA3n
-                        para hoy                        09 de Agosto de 2023
-Atras quedaron los dias en los que se consideraba que aquellas personas que creian en las hadas y la magia eran unas credulas. Avanzando en el tiempo, no hace mucho se consideraba credula a la gente que creia en el calentamiento global. No es mi intencion transmitir una opinion. Simplemente estoy senalando que, sean cuales sean nuestras teorias y creencias, corremos el riesgo de que se burlen de ellas. Y que cuando una persona a la que valoramos critica nuestros puntos de vista, esto puede hacer que dudemos. Hoy no dejes que te convenzan de algo. Tus ideas estan bien pensadas y son validas. Merecen que obres en consecuencia.</t>
+                        para hoy                        15 de Agosto de 2023
+Donde otras personas ven montanas que superar, tu ves soluciones. Cuando los demas estamos aturdidos y desconcertados, tu puedes encontrar el camino a traves de la confusion. Lo frustrante es que tus soluciones no siempre son bien recibidas. Por desgracia, solo porque tu lo veas claro, no significa que los otros esten dispuestos a seguirte. Asi que el hecho de que todo el mundo te pida consejo (y tu no sepas que hacer) es poco habitual, por no decir inquietante. Lo que era oscuro se aclarara bajo el influjo de la oscuridad de la Luna - y tu solucion te impresionara incluso a ti.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Lo malo de las nuevas ideas es que exigen un cambio de actitud. Ponerlas en practica significa reajustar las expectativas y alterar las rutinas. Lo cual esta bien cuando somos nosotros los promotores de la idea. Pero cuando viene de otra persona es mas dificil y tendemos a considerarla una molestia. Ademas tenemos problemas con las ideas que nacen de la necesidad (en lugar de la inspiracion). Sin embargo, venga de donde venga una idea, merece la pena investigarla bajo el influjo de la oscuridad de la Luna. Estate abierta a lo que venga. Una idea que descartarias facilmente podria ser revolucionaria.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Es como si estuvieras intentando montar un puzle sin tener la foto como guia. O como armar un mueble sin tener las instrucciones. Ni siquiera estas segura de si son las piezas correctas porque, hagas lo que hagas, las que tienes no parecen encajar entre si. !Que rabia! Mira que es frustrante. Pero tienes que seguir experimentando. No pierdas el optimismo. Puedes encontrar la respuesta a tu pregunta probando, equivocandote, mejorando y usando tu ingenio. Y una vez que la hayas encontrado, sabras que hacer exactamente para mejorar tus circunstancias actuales. !Sigue adelante!</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+La oscuridad de la Luna es un momento poderoso para ti. Como tu regente casi desaparece de los cielos, tus emociones se intensifican. Experimentas sentimientos profundos. Tus experiencias te parecen mas extremas. Lo que significa que las oportunidades te dan miedo. Pero estos sintomas son positivos. Te estan resultando muy saludables. Estas plantando cara a tus temores y venciendo tus inhibiciones. Asi que se valiente y centrate en esas dificultades. Estas al borde de un gran avance. Las repercusiones podrian suponer un cambio que sera beneficioso durante mucho tiempo.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Si tuvieras una maquina del tiempo, ?que harias? ?A que acontecimientos de tu pasado viajarias para cambiarlos? ?Que consejo le darias a tu antiguo yo? ?Tienes algun truco o idea que transmitirle? ?Algunas palabras de consuelo y aliento? A pesar de nuestros avances tecnicos, no se ha inventado ningun dispositivo de este tipo. Sin embargo, a medida que nos acercamos a la Luna Nueva (que sera en tu signo) algo con lo que nunca te has atrevido a sonar esta lo suficientemente cerca como para poder tocarlo. Algo imposible se esta haciendo posible. Tu perspectiva de futuro puede transformarse.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Si no te importa olvidar todo lo que te hayan contado acerca de la famosa capacidad para discernir que teneis los nativos de Virgo y vuestra minuciosidad, seria un signo perfecto. No es que esta imagen sea falsa... pero desde luego no esta completa. Y corres el peligro de que, al sentirte presionada a ajustarte a ciertas expectativas, puedas acabar quitando el brillo a tus otras cualidades, ocultandolas bajo una capa de modestia. La oscuridad de la Luna fomenta tu lado creativo y tu caracter desbordante de vida y entusiasmo. No te costaria nada dejar que las exigencias de los demas se interpusieran en tu camino. No lo permitas.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Lo que es importante para mi puede no serlo para ti. Que a mi me guste la pizza no significa que a ti tambien te guste. Lo que para mi puede ser una crisis, para ti puede ser un simple contratiempo. Sabemos esto. Pero se nos olvida. Por lo que sea, pensamos que todo el mundo siente y piensa igual que nosotros. Y luego nos preguntamos por que nadie nos comprende. Cierta persona de tu mundo esta tan interesada en que entiendas su punto de vista que hace todo lo posible por compartirlo contigo. Ten con ella toda la paciencia de que seas capaz. Significa mucho para ella. Hasta es posible acabe siendo importante para ti.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Si estas corriendo y ya llevas una pelota, va a ser todo un reto para ti coger otra pelota que casualmente rueda en tu direccion. ?Deberias soltar la primera? ?Como vas a saber a cual te conviene aferrarte: a la que ya tienes o a la que podrias tener si no hubieras cogido la otra antes? Vaya pregunta... es dificil dar una respuesta. Procura no confundir mas las cosas, dejando que te preocupe lo que piensen los demas. Ni tampoco dejes que te influya un equivocado sentido de la lealtad. Se justa. Pero no seas sentimental.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+"La esperanza es esa cosa con plumas que se posa en el alma". Cito estas sabias palabras porque estas contemplando dejar aparcada una idea que podria estar a punto de alzar el vuelo. Nadie quiere sentirse decepcionado. Pero cerrarte a la oportunidad de poner en marcha un cambio, no cambiara nada. No puedes quedarte quieta y tampoco quieres hacerlo. Por supuesto que dar el primer paso te produce temor. Hara que te sientas vulnerable. Pero si eres lo bastante valiente como para desplegar tus alas, enseguida estaras volando mas alto de lo que te atreviste a sonar.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+"?Juras decir toda la verdad y nada mas que la verdad?" !Esto si que es un reto! Puede parecer sencillo. Pero si tu y yo somos testigos del mismo suceso, cada uno le daremos, sin proponernoslo, nuestro propio giro a la historia. No es que queramos faltar a la verdad, pero no podemos evitar verlo a traves de nuestros ojos, lo que significa que nuestra experiencia (antes, durante e incluso despues del suceso) influye en nuestra version. Hoy ten esto en cuenta cuando intentes tomar una decision basandote en la version que ha dado otra persona de lo que ha pasado. No partas de ideas preconcebidas.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Es facil idealizar a la gente que nos importa. Pensar en su cuidado y apoyo puede emocionarnos. Pero luego esta !la realidad! Solo tenemos que pasar un rato en su compania para recordar sus extranas y molestas costumbres. Nos resulto muy comodo olvidar los rasgos de su caracter que nos sacaban de quicio. Pero eso no significa que los queramos menos. En la oscuridad de la Luna tienes que adaptarte a una realidad que no se ajusta a una fantasia. Pero ver a otra persona tal y como es en realidad tiene sus recompensas. Puede haber una conexion interesante.</t>
+  </si>
+  <si>
+    <t>PredicciA3n
+                        para hoy                        15 de Agosto de 2023
+Hay muchas cosas que nunca llegaremos a saber. Entre ellas estan las que creemos saber (pero que desconocemos). Hacemos conjeturas basandonos en informacion erronea y despues amontonamos capas de logica encima de ellas. Luego nos preguntamos por que las cosas no nos salen como habiamos planeado. Es un milagro que esto no ocurra mas a menudo. Estas reestructurando un plan para tu futuro. Es todo un reto. Pero si aplicas todo lo que has aprendido y la experiencia adquirida hasta ahora, construiras un camino a seguir con cimientos solidos que perduraran en el tiempo.</t>
   </si>
   <si>
     <t>https://www.hola.com/horoscopo/aries/</t>

</xml_diff>